<commit_message>
splitting out stepper and servo
</commit_message>
<xml_diff>
--- a/9-12-2020-Desk.xlsx
+++ b/9-12-2020-Desk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colton\Documents\Projects\SkittleSorter\Skittles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4643F5-1CF4-4C1D-B355-D75B814FE9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78211D97-FEF9-4AB3-BED6-1970481CCBBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4545" windowWidth="21600" windowHeight="14640" activeTab="1" xr2:uid="{ED2ABE13-5B7A-49C2-BB65-DE205F600B8A}"/>
   </bookViews>
@@ -24,6 +24,8 @@
     <definedName name="_xlchart.v1.11" hidden="1">Dark!$C$2:$C$39</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">Dark!$D$1</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">Dark!$D$2:$D$39</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Dark!$E$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Dark!$E$2:$E$39</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Fair Lighting'!$B$2:$B$23</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Fair Lighting'!$C$1</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Fair Lighting'!$C$2:$C$23</definedName>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="14">
   <si>
     <t>Red</t>
   </si>
@@ -90,6 +92,9 @@
   </si>
   <si>
     <t>Average Blue</t>
+  </si>
+  <si>
+    <t>Mean Squared Error</t>
   </si>
 </sst>
 </file>
@@ -131,7 +136,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -284,6 +293,14 @@
         <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
+    <cx:data id="3">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:title pos="t" align="ctr" overlay="0">
@@ -352,6 +369,18 @@
           <cx:dataId val="2"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{5D68E813-6F60-456C-BB4C-A159D26D8E7B}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>Mean Squared Error</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -1567,16 +1596,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>214311</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1062036</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1612,7 +1641,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3995736" y="2333625"/>
+              <a:off x="5729286" y="2257425"/>
               <a:ext cx="5624513" cy="3009900"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1647,13 +1676,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EAC82E7-7334-4615-ADD7-BFDC2691C8AF}" name="Table1" displayName="Table1" ref="A1:D39" totalsRowShown="0">
-  <autoFilter ref="A1:D39" xr:uid="{F20983AC-2265-4EE1-B1C6-1E8A03CFCB4C}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EAC82E7-7334-4615-ADD7-BFDC2691C8AF}" name="Table1" displayName="Table1" ref="A1:E39" totalsRowShown="0">
+  <autoFilter ref="A1:E39" xr:uid="{F20983AC-2265-4EE1-B1C6-1E8A03CFCB4C}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{32F98D35-56E3-4041-8FE2-601A7FF563C5}" name="Skittle Color"/>
     <tableColumn id="2" xr3:uid="{6525C656-C636-4826-9165-93F09C531988}" name="Red"/>
     <tableColumn id="3" xr3:uid="{20A1669A-4328-4AF4-95FC-11F3459CA59D}" name="Green"/>
     <tableColumn id="4" xr3:uid="{9EFCBF4C-AAA0-43D1-A43E-3ED8A34488C9}" name="Blue"/>
+    <tableColumn id="5" xr3:uid="{30A30316-C740-4BD3-8C0B-482E110BD853}" name="Mean Squared Error" dataDxfId="0">
+      <calculatedColumnFormula>SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2291,10 +2323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D58605-98B7-4F62-9E56-044C48AE10B4}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,7 +2336,7 @@
     <col min="8" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2317,17 +2349,20 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2340,23 +2375,31 @@
       <c r="D2">
         <v>186</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.8989794855663558</v>
+      </c>
+      <c r="G2">
+        <f>SQRT((159-155)^2+(214-212)^2+(184-186)^2)</f>
+        <v>4.8989794855663558</v>
+      </c>
+      <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="G2">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F2,Table1[Red]),0)</f>
+      <c r="I2">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H2,Table1[Red]),0)</f>
         <v>155</v>
       </c>
-      <c r="H2">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F2,Table1[Green]),0)</f>
+      <c r="J2">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H2,Table1[Green]),0)</f>
         <v>212</v>
       </c>
-      <c r="I2">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F2,Table1[Blue]),0)</f>
+      <c r="K2">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H2,Table1[Blue]),0)</f>
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2369,23 +2412,27 @@
       <c r="D3">
         <v>187</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="G3">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F3,Table1[Red]),0)</f>
+      <c r="I3">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H3,Table1[Red]),0)</f>
         <v>146</v>
       </c>
-      <c r="H3">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F3,Table1[Green]),0)</f>
+      <c r="J3">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H3,Table1[Green]),0)</f>
         <v>232</v>
       </c>
-      <c r="I3">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F3,Table1[Blue]),0)</f>
+      <c r="K3">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H3,Table1[Blue]),0)</f>
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2398,23 +2445,27 @@
       <c r="D4">
         <v>182</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="G4">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F4,Table1[Red]),0)</f>
+      <c r="I4">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H4,Table1[Red]),0)</f>
         <v>137</v>
       </c>
-      <c r="H4">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F4,Table1[Green]),0)</f>
+      <c r="J4">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H4,Table1[Green]),0)</f>
         <v>209</v>
       </c>
-      <c r="I4">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F4,Table1[Blue]),0)</f>
+      <c r="K4">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H4,Table1[Blue]),0)</f>
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2427,23 +2478,27 @@
       <c r="D5">
         <v>183</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="G5">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F5,Table1[Red]),0)</f>
+      <c r="I5">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H5,Table1[Red]),0)</f>
         <v>187</v>
       </c>
-      <c r="H5">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F5,Table1[Green]),0)</f>
+      <c r="J5">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H5,Table1[Green]),0)</f>
         <v>224</v>
       </c>
-      <c r="I5">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F5,Table1[Blue]),0)</f>
+      <c r="K5">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H5,Table1[Blue]),0)</f>
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2456,23 +2511,27 @@
       <c r="D6">
         <v>182</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
         <v>5</v>
       </c>
-      <c r="G6">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F6,Table1[Red]),0)</f>
+      <c r="I6">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H6,Table1[Red]),0)</f>
         <v>198</v>
       </c>
-      <c r="H6">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F6,Table1[Green]),0)</f>
+      <c r="J6">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H6,Table1[Green]),0)</f>
         <v>255</v>
       </c>
-      <c r="I6">
-        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$F6,Table1[Blue]),0)</f>
+      <c r="K6">
+        <f ca="1">ROUND(AVERAGEIF($A$2:$D$39,$H6,Table1[Blue]),0)</f>
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2485,8 +2544,12 @@
       <c r="D7">
         <v>189</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>3.4641016151377544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2499,8 +2562,12 @@
       <c r="D8">
         <v>184</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2513,8 +2580,12 @@
       <c r="D9">
         <v>189</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.4721359549995796</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2527,8 +2598,12 @@
       <c r="D10">
         <v>188</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2541,8 +2616,12 @@
       <c r="D11">
         <v>199</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2555,8 +2634,12 @@
       <c r="D12">
         <v>184</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2569,8 +2652,12 @@
       <c r="D13">
         <v>185</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2583,8 +2670,12 @@
       <c r="D14">
         <v>186</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2597,8 +2688,12 @@
       <c r="D15">
         <v>188</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2611,8 +2706,12 @@
       <c r="D16">
         <v>182</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2625,8 +2724,12 @@
       <c r="D17">
         <v>188</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2639,8 +2742,12 @@
       <c r="D18">
         <v>191</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.8989794855663558</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2653,8 +2760,12 @@
       <c r="D19">
         <v>201</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>9.2195444572928871</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2667,8 +2778,12 @@
       <c r="D20">
         <v>186</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.2426406871192848</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2681,8 +2796,12 @@
       <c r="D21">
         <v>185</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2695,8 +2814,12 @@
       <c r="D22">
         <v>191</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.8989794855663558</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2709,8 +2832,12 @@
       <c r="D23">
         <v>187</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>3.6055512754639891</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2723,8 +2850,12 @@
       <c r="D24">
         <v>183</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2737,8 +2868,12 @@
       <c r="D25">
         <v>187</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2751,8 +2886,12 @@
       <c r="D26">
         <v>188</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>5.4772255750516612</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2765,8 +2904,12 @@
       <c r="D27">
         <v>183</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -2779,8 +2922,12 @@
       <c r="D28">
         <v>181</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -2793,8 +2940,12 @@
       <c r="D29">
         <v>191</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>8.1240384046359608</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2807,8 +2958,12 @@
       <c r="D30">
         <v>187</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.5825756949558398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -2821,8 +2976,12 @@
       <c r="D31">
         <v>180</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>3.4641016151377544</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -2835,8 +2994,12 @@
       <c r="D32">
         <v>181</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2849,8 +3012,12 @@
       <c r="D33">
         <v>188</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>8.6023252670426267</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -2863,8 +3030,12 @@
       <c r="D34">
         <v>181</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>1.7320508075688772</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2877,8 +3048,12 @@
       <c r="D35">
         <v>187</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2891,8 +3066,12 @@
       <c r="D36">
         <v>188</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2905,8 +3084,12 @@
       <c r="D37">
         <v>184</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>9.8994949366116654</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2919,8 +3102,12 @@
       <c r="D38">
         <v>182</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>3.4641016151377544</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2932,6 +3119,10 @@
       </c>
       <c r="D39">
         <v>187</v>
+      </c>
+      <c r="E39">
+        <f ca="1">SQRT((Table1[[#This Row],[Red]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$I$6,2,FALSE))^2+(Table1[[#This Row],[Green]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,3,FALSE))^2+(Table1[[#This Row],[Blue]]-VLOOKUP(Table1[[#This Row],[Skittle Color]],$H$2:$K$6,4,FALSE))^2)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>